<commit_message>
Updated example file - Header row
</commit_message>
<xml_diff>
--- a/data/Account_Information_PPL.xlsx
+++ b/data/Account_Information_PPL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\CEToolBox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352C09CF-081B-4320-BF61-D5A86998CEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08D0FCC-F49F-451D-BB14-A2B96E3455B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="855" windowWidth="22005" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Months</t>
   </si>
@@ -50,9 +50,6 @@
     <t>ACCOUNT NAME</t>
   </si>
   <si>
-    <t>LINE 2</t>
-  </si>
-  <si>
     <t>SERVICE ADDRESS LINE 1</t>
   </si>
   <si>
@@ -297,6 +294,15 @@
   </si>
   <si>
     <t>G100</t>
+  </si>
+  <si>
+    <t>ALINE 2</t>
+  </si>
+  <si>
+    <t>SLINE 2</t>
+  </si>
+  <si>
+    <t>BLINE 2</t>
   </si>
 </sst>
 </file>
@@ -642,7 +648,7 @@
   <dimension ref="A1:CE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,229 +670,229 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AA1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:83" x14ac:dyDescent="0.25">
@@ -900,40 +906,40 @@
         <v>213020</v>
       </c>
       <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>81</v>
-      </c>
-      <c r="I2" t="s">
-        <v>82</v>
       </c>
       <c r="J2">
         <v>12345</v>
       </c>
       <c r="L2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
         <v>83</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>84</v>
-      </c>
-      <c r="O2" t="s">
-        <v>85</v>
       </c>
       <c r="P2">
         <v>67891</v>
       </c>
       <c r="R2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:83" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated default excel file
</commit_message>
<xml_diff>
--- a/data/Account_Information_PPL.xlsx
+++ b/data/Account_Information_PPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\CEToolBox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08D0FCC-F49F-451D-BB14-A2B96E3455B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364EFED3-38BF-42D6-8EFC-BE11BC0C4142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="855" windowWidth="22005" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,6 @@
     <t>TX</t>
   </si>
   <si>
-    <t>99 Shoot</t>
-  </si>
-  <si>
     <t>The City</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>BLINE 2</t>
+  </si>
+  <si>
+    <t>99 Trench Market</t>
   </si>
 </sst>
 </file>
@@ -357,14 +357,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE3"/>
+  <dimension ref="A1:CE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,13 +667,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -691,7 +688,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
@@ -927,30 +924,20 @@
         <v>12345</v>
       </c>
       <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" t="s">
         <v>82</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>83</v>
-      </c>
-      <c r="O2" t="s">
-        <v>84</v>
       </c>
       <c r="P2">
         <v>67891</v>
       </c>
       <c r="R2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>